<commit_message>
Update catch-certificate-report.xlsx template to show only TUR catches
</commit_message>
<xml_diff>
--- a/templates/export/catch-certificate-report.xlsx
+++ b/templates/export/catch-certificate-report.xlsx
@@ -35,7 +35,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:area(lastCell="S11")</t>
+          <t xml:space="preserve">jx:area(lastCell="T11")</t>
         </r>
       </text>
     </comment>
@@ -49,7 +49,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="devices", var="device", lastCell="S11" multisheet="sheetNames")</t>
+          <t xml:space="preserve">jx:each(items="devices", var="device", lastCell="T11" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
@@ -61,8 +61,9 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="device.objects", var="position", lastCell="S11")</t>
+          <t xml:space="preserve">jx:each(items="device.objects", var="position", lastCell="T11")</t>
         </r>
       </text>
     </comment>
@@ -74,8 +75,39 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="position.catches" var="catch" lastCell="S11")</t>
+          <t xml:space="preserve">jx:each(items="position.catches" var="catch" lastCell="T11")
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    jx:if(condition="catch.</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF333333"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">speciesCode == </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">'TUR'" lastCell="T11" )
+    /jx:if
+/jx:each</t>
         </r>
       </text>
     </comment>
@@ -84,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t xml:space="preserve">Отчет:</t>
   </si>
@@ -137,6 +169,9 @@
     <t xml:space="preserve">Оценено живо тегло (кг)</t>
   </si>
   <si>
+    <t xml:space="preserve">Код на улова</t>
+  </si>
+  <si>
     <t xml:space="preserve">Дата на улов</t>
   </si>
   <si>
@@ -207,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve">${catch.speciesWeightKilograms}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${catch.speciesCode}</t>
   </si>
   <si>
     <t xml:space="preserve">${dateTool.format("DD.MM.YYYY", catch.endFishingOperationDateTime, locale, timezone)}</t>
@@ -233,7 +271,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -284,6 +322,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -313,6 +352,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -320,6 +360,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -330,16 +371,22 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -420,10 +467,8 @@
       <right style="thin">
         <color rgb="FFCCCCCC"/>
       </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin"/>
+      <top style="thin"/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -433,10 +478,8 @@
       <right style="thin">
         <color rgb="FFCCCCCC"/>
       </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin"/>
+      <top style="thin"/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -477,7 +520,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -578,7 +621,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -590,15 +633,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -606,7 +641,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -694,9 +729,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
+      <xdr:colOff>1268280</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -706,7 +741,97 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9843840" cy="9523800"/>
+          <a:ext cx="9841320" cy="9523440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1268280</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9841320" cy="9523440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1268280</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9841320" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -745,103 +870,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9843840" cy="9523800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9843840" cy="9523800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1269000</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="shapetype_202" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9844200" cy="9524160"/>
+          <a:ext cx="9841680" cy="9523800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -874,9 +909,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1269000</xdr:colOff>
+      <xdr:colOff>1268640</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -886,7 +921,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9844200" cy="9524160"/>
+          <a:ext cx="9841680" cy="9523800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -919,9 +954,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1269000</xdr:colOff>
+      <xdr:colOff>1268640</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>81720</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -931,7 +966,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9844200" cy="9524160"/>
+          <a:ext cx="9841680" cy="9523800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -963,31 +998,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ17"/>
+  <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="14" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1109,66 +1144,68 @@
       <c r="P8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="Q8" s="13"/>
+      <c r="Q8" s="13" t="s">
+        <v>19</v>
+      </c>
       <c r="R8" s="13"/>
       <c r="S8" s="13"/>
-      <c r="T8" s="0"/>
+      <c r="T8" s="13"/>
       <c r="U8" s="0"/>
-      <c r="AMI8" s="0"/>
-      <c r="AMJ8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
     </row>
     <row r="9" s="14" customFormat="true" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="F9" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="16" t="s">
-        <v>23</v>
-      </c>
       <c r="M9" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
-      <c r="P9" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q9" s="18" t="s">
+      <c r="P9" s="13"/>
+      <c r="Q9" s="17" t="s">
         <v>26</v>
       </c>
       <c r="R9" s="18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="S9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="0"/>
+      <c r="T9" s="18" t="s">
+        <v>27</v>
+      </c>
       <c r="U9" s="0"/>
-      <c r="AMI9" s="0"/>
-      <c r="AMJ9" s="0"/>
+      <c r="V9" s="0"/>
+      <c r="W9" s="0"/>
     </row>
     <row r="10" s="14" customFormat="true" ht="8.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="19"/>
@@ -1186,89 +1223,91 @@
       <c r="M10" s="21"/>
       <c r="N10" s="22"/>
       <c r="O10" s="22"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="23"/>
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
-      <c r="T10" s="0"/>
+      <c r="T10" s="22"/>
       <c r="U10" s="0"/>
-      <c r="AMI10" s="0"/>
-      <c r="AMJ10" s="0"/>
+      <c r="V10" s="0"/>
+      <c r="W10" s="0"/>
     </row>
-    <row r="11" s="31" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" s="29" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I11" s="26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="K11" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="M11" s="28" t="s">
+      <c r="L11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="26" t="s">
+      <c r="M11" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="O11" s="29" t="s">
+      <c r="N11" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="30" t="s">
+      <c r="O11" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="Q11" s="30" t="s">
+      <c r="P11" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="R11" s="30" t="s">
+      <c r="Q11" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="S11" s="30" t="s">
+      <c r="R11" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="T11" s="0"/>
+      <c r="S11" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="T11" s="26" t="s">
+        <v>47</v>
+      </c>
       <c r="U11" s="0"/>
-      <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
+      <c r="V11" s="0"/>
+      <c r="W11" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:D8"/>
@@ -1279,7 +1318,8 @@
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:T8"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
In catchCertificate.vm updated filter for TUR
</commit_message>
<xml_diff>
--- a/templates/export/catch-certificate-report.xlsx
+++ b/templates/export/catch-certificate-report.xlsx
@@ -63,7 +63,12 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t xml:space="preserve">jx:each(items="device.objects", var="position", lastCell="T11")</t>
+          <t xml:space="preserve">jx:each(items="device.objects", var="position", lastCell="T11")
+    jx:each(items="position.catches" var="catch" lastCell="T11")
+        jx:if(condition="catch.speciesCode == 'TUR'" lastCell="T11" )
+        /jx:if
+    /jx:each
+ /jx:each</t>
         </r>
       </text>
     </comment>
@@ -86,6 +91,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">    jx:if(condition="catch.</t>
         </r>
@@ -95,6 +101,7 @@
             <color rgb="FF333333"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">speciesCode == </t>
         </r>
@@ -104,6 +111,7 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">'TUR'" lastCell="T11" )
     /jx:if
@@ -271,7 +279,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -375,18 +383,6 @@
       <name val="Courier New"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -729,9 +725,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1268280</xdr:colOff>
+      <xdr:colOff>1267920</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
+      <xdr:rowOff>80640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -741,7 +737,97 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9841320" cy="9523440"/>
+          <a:ext cx="9840600" cy="9523080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1267920</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>80640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9840600" cy="9523080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1267920</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>80640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9840600" cy="9523080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -780,103 +866,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9841320" cy="9523440"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1268280</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>81000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9841320" cy="9523440"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="shapetype_202" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9841680" cy="9523800"/>
+          <a:ext cx="9840960" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -909,9 +905,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
+      <xdr:colOff>1268280</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -921,7 +917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9841680" cy="9523800"/>
+          <a:ext cx="9840960" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -954,9 +950,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1268640</xdr:colOff>
+      <xdr:colOff>1268280</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>81360</xdr:rowOff>
+      <xdr:rowOff>81000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -966,7 +962,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9841680" cy="9523800"/>
+          <a:ext cx="9840960" cy="9523440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1000,18 +996,18 @@
   </sheetPr>
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.2"/>

</xml_diff>